<commit_message>
main assignment some rating part added
</commit_message>
<xml_diff>
--- a/Main_Assignment/PythonData.xlsx
+++ b/Main_Assignment/PythonData.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -401,10 +401,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -465,49 +465,76 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>rav</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ravi123</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>123</v>
+      </c>
+      <c r="E7" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>ravi</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ravi</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" t="n">
-        <v>4564</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ravi@gmail.com</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ravi123</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>123</v>
+      </c>
+      <c r="E8" t="n">
+        <v>23</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ravi</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>ravi123@gmail.com</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>678</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>rav</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>rav@gmail.com</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>123</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E9" t="n">
         <v>23</v>
       </c>
     </row>

</xml_diff>